<commit_message>
Updated test framework, features, and runner for Jenkins execution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\eclipsenew\Team3_RestAssuredNinjas\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4F29A9-CA72-4664-94D5-E7DCCB4C6A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D84EF-2E90-4D62-85BF-A0909EB14F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A614770-2B86-4A76-AD6E-273504CE2649}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>TestcaseId</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>posrRePwdwrongEmail</t>
+  </si>
+  <si>
+    <t>ApiHackathona2@3</t>
+  </si>
+  <si>
+    <t>postresetPwdWrongEnd</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453E46AD-BC29-4854-805E-E5E6990D020B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,12 +674,12 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -697,6 +703,17 @@
       </c>
       <c r="C17" s="7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -708,11 +725,12 @@
     <hyperlink ref="B7" r:id="rId5" display="mailto:team3@gmail.com" xr:uid="{3CFF8147-F27F-436C-A1D1-3B25021EABD2}"/>
     <hyperlink ref="B10" r:id="rId6" display="mailto:team3@gmail.com" xr:uid="{F331228F-3003-45C6-95C7-AD2A47AC55A1}"/>
     <hyperlink ref="B14" r:id="rId7" display="mailto:team3@gmail.com" xr:uid="{4CF33C01-35ED-4134-9487-EEC23B3A0042}"/>
-    <hyperlink ref="B15" r:id="rId8" display="mailto:team3@gmail.com" xr:uid="{9AE9A746-CC42-473F-A0DB-83AEE6C3BD94}"/>
-    <hyperlink ref="C15" r:id="rId9" xr:uid="{8DAC0E1D-2176-48FE-8B53-6FAE3741380E}"/>
+    <hyperlink ref="B18" r:id="rId8" display="mailto:team3@gmail.com" xr:uid="{9AE9A746-CC42-473F-A0DB-83AEE6C3BD94}"/>
+    <hyperlink ref="C18" r:id="rId9" xr:uid="{8DAC0E1D-2176-48FE-8B53-6FAE3741380E}"/>
     <hyperlink ref="B16" r:id="rId10" xr:uid="{A92CFD70-A8AB-47E1-AFBF-0F3BA7690514}"/>
     <hyperlink ref="B17" r:id="rId11" xr:uid="{3D6C142C-C020-492A-B5CF-87F1E4A30EB4}"/>
     <hyperlink ref="C17" r:id="rId12" xr:uid="{825624C5-DB65-482E-AD68-CD2AE98AF5FB}"/>
+    <hyperlink ref="B15" r:id="rId13" display="mailto:team3@gmail.com" xr:uid="{5DE07759-A341-48E5-932D-CFBA354DC1FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>